<commit_message>
Cleanup - main.py is now main optimization model
</commit_message>
<xml_diff>
--- a/Test battery data.xlsx
+++ b/Test battery data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-7440" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NO1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NO3" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NO4" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPARE" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="NO1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NO3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NO4" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="COMPARE" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -208,14 +208,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -238,8 +238,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -265,7 +265,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -276,7 +276,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -451,7 +451,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -462,7 +462,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -637,7 +637,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -648,7 +648,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -823,7 +823,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -834,7 +834,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -1016,9 +1016,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -1041,8 +1041,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1053,8 +1053,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1066,9 +1066,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -1104,7 +1104,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -1119,9 +1119,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -1144,8 +1144,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1156,16 +1156,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -1194,16 +1194,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1231,14 +1231,14 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1261,8 +1261,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1288,7 +1288,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1299,7 +1299,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -1474,7 +1474,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1485,7 +1485,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -1667,9 +1667,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -1692,8 +1692,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1704,8 +1704,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1717,9 +1717,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -1755,7 +1755,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -1770,9 +1770,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -1795,8 +1795,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1807,16 +1807,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -1845,16 +1845,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1882,14 +1882,14 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1912,8 +1912,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1939,7 +1939,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1950,7 +1950,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -2125,7 +2125,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -2136,7 +2136,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -2311,7 +2311,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -2322,7 +2322,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -2513,7 +2513,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -2524,7 +2524,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -2707,9 +2707,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -2732,8 +2732,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -2743,8 +2743,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -2756,9 +2756,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -2794,7 +2794,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -2809,9 +2809,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -2834,8 +2834,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -2846,16 +2846,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -2906,9 +2906,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -2935,8 +2935,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -2947,16 +2947,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -2985,16 +2985,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -3022,14 +3022,14 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:r>
               <a:rPr lang="nb-NO"/>
               <a:t>None</a:t>
@@ -3039,8 +3039,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -3066,7 +3066,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -3077,7 +3077,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -3268,7 +3268,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -3279,7 +3279,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -3464,8 +3464,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -3477,9 +3477,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -3515,7 +3515,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -3532,16 +3532,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -3594,16 +3594,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -3632,16 +3632,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -3669,14 +3669,14 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -3699,8 +3699,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -3726,7 +3726,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -3737,7 +3737,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -3912,7 +3912,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -3923,7 +3923,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -4098,7 +4098,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -4109,7 +4109,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -4291,9 +4291,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -4316,8 +4316,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -4328,8 +4328,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -4341,9 +4341,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -4379,7 +4379,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -4394,9 +4394,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -4419,8 +4419,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -4431,16 +4431,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -4469,16 +4469,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -4506,14 +4506,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -4536,8 +4536,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -4563,7 +4563,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -4574,7 +4574,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -4749,7 +4749,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -4760,7 +4760,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -4942,9 +4942,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -4967,8 +4967,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -4979,8 +4979,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -4992,9 +4992,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -5030,7 +5030,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -5045,9 +5045,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -5070,8 +5070,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -5082,16 +5082,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -5120,16 +5120,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -5157,14 +5157,14 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -5187,8 +5187,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -5214,7 +5214,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -5225,7 +5225,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -5400,7 +5400,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -5411,7 +5411,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -5586,7 +5586,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -5597,7 +5597,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -5788,7 +5788,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -5799,7 +5799,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -5982,9 +5982,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -6007,8 +6007,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -6019,8 +6019,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -6032,9 +6032,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6070,7 +6070,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -6085,9 +6085,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -6110,8 +6110,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -6122,16 +6122,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6182,9 +6182,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -6211,8 +6211,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -6223,16 +6223,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6261,16 +6261,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -6298,14 +6298,14 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:r>
               <a:t>None</a:t>
             </a:r>
@@ -6314,8 +6314,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -6341,7 +6341,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -6352,7 +6352,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -6543,7 +6543,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -6554,7 +6554,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -6738,8 +6738,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -6751,9 +6751,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6789,7 +6789,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -6806,16 +6806,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6868,16 +6868,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -6906,16 +6906,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -6943,14 +6943,14 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -6973,8 +6973,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -7000,7 +7000,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -7011,7 +7011,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -7186,7 +7186,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -7197,7 +7197,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -7372,7 +7372,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -7383,7 +7383,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -7558,7 +7558,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -7569,7 +7569,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -7751,9 +7751,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
                 <a:r>
                   <a:rPr lang="nb-NO" sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -7773,8 +7773,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -7785,8 +7785,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -7798,9 +7798,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -7836,7 +7836,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -7851,9 +7851,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
                 <a:r>
                   <a:rPr lang="nb-NO" sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -7873,8 +7873,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -7885,16 +7885,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -7923,16 +7923,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -7960,14 +7960,14 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -7990,8 +7990,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -8017,7 +8017,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -8028,7 +8028,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -8203,7 +8203,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -8214,7 +8214,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -8396,9 +8396,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -8421,8 +8421,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -8433,8 +8433,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -8446,9 +8446,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -8484,7 +8484,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -8499,9 +8499,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -8524,8 +8524,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -8536,16 +8536,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -8574,16 +8574,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -8611,14 +8611,14 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -8641,8 +8641,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -8668,7 +8668,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -8679,7 +8679,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -8854,7 +8854,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -8865,7 +8865,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9040,7 +9040,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -9051,7 +9051,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9242,7 +9242,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -9253,7 +9253,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9436,9 +9436,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -9461,8 +9461,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -9473,8 +9473,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -9486,9 +9486,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -9524,7 +9524,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -9539,9 +9539,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -9564,8 +9564,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -9576,16 +9576,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -9636,9 +9636,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -9665,8 +9665,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -9677,16 +9677,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -9715,16 +9715,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -9752,14 +9752,14 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:r>
               <a:rPr lang="nb-NO"/>
               <a:t>None</a:t>
@@ -9769,8 +9769,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -9796,7 +9796,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -9807,7 +9807,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9998,7 +9998,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -10009,7 +10009,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -10193,8 +10193,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -10206,9 +10206,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -10244,7 +10244,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -10261,16 +10261,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -10323,16 +10323,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -10361,16 +10361,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -10398,14 +10398,14 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -10429,8 +10429,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -10456,7 +10456,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -10467,7 +10467,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -10642,7 +10642,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -10653,7 +10653,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -10828,7 +10828,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -10839,7 +10839,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -11014,7 +11014,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -11025,7 +11025,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -11207,9 +11207,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -11232,8 +11232,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -11244,8 +11244,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -11257,9 +11257,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -11295,7 +11295,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -11310,9 +11310,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
@@ -11335,8 +11335,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -11347,16 +11347,16 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
@@ -11385,16 +11385,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -11422,7 +11422,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>9</col>
@@ -11442,9 +11442,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11469,9 +11469,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11496,9 +11496,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11523,9 +11523,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11535,7 +11535,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>9</col>
@@ -11555,9 +11555,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11582,9 +11582,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11609,9 +11609,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11636,9 +11636,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11648,7 +11648,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>9</col>
@@ -11668,9 +11668,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11695,9 +11695,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11722,9 +11722,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11749,9 +11749,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -11761,7 +11761,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>4</col>
@@ -11781,9 +11781,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -12076,7 +12076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -30866,12 +30866,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -49661,12 +49661,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -68456,12 +68456,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -78577,6 +78577,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>